<commit_message>
better reg design, improved nullmove and added d1 futility pruning
</commit_message>
<xml_diff>
--- a/src/regressions.xlsx
+++ b/src/regressions.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\github\chess\viridithas_chess\src\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A0D05B8-CEF1-4247-ACBD-9DAE032DEC4C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A58FDF5-D365-4FCE-A3EA-D4694AC2DE1D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{D29FE3B1-2868-4402-B04C-E409A12BF9BB}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="16">
   <si>
     <t>ALL_COMPONENTS</t>
   </si>
@@ -64,6 +64,24 @@
   </si>
   <si>
     <t>SPACE</t>
+  </si>
+  <si>
+    <t>6a60558f6bbb81c9558168487227b3f69e6ac010</t>
+  </si>
+  <si>
+    <t>SEE</t>
+  </si>
+  <si>
+    <t>FUTILITY</t>
+  </si>
+  <si>
+    <t>NEW_FUTILITY</t>
+  </si>
+  <si>
+    <t>RAW_EVAL</t>
+  </si>
+  <si>
+    <t>NULLWINDOW_NULLMOVE</t>
   </si>
 </sst>
 </file>
@@ -178,6 +196,17 @@
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$B$13</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>ALL_COMPONENTS</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
           <c:spPr>
             <a:ln w="19050" cap="rnd">
               <a:solidFill>
@@ -204,7 +233,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$A$12:$A$15</c:f>
+              <c:f>Sheet1!$A$14:$A$17</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
@@ -225,7 +254,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$B$12:$B$15</c:f>
+              <c:f>Sheet1!$B$14:$B$17</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="4"/>
@@ -247,13 +276,24 @@
           <c:smooth val="1"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-A2A6-48AE-957B-318FFA22B2E9}"/>
+              <c16:uniqueId val="{00000000-BD17-4B80-85E9-6720A4C194FF}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
           <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$C$13</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>ONLY_PST</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
           <c:spPr>
             <a:ln w="19050" cap="rnd">
               <a:solidFill>
@@ -280,7 +320,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$A$12:$A$15</c:f>
+              <c:f>Sheet1!$A$14:$A$17</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
@@ -301,7 +341,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$C$12:$C$15</c:f>
+              <c:f>Sheet1!$C$14:$C$17</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="4"/>
@@ -323,7 +363,436 @@
           <c:smooth val="1"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-A2A6-48AE-957B-318FFA22B2E9}"/>
+              <c16:uniqueId val="{00000001-BD17-4B80-85E9-6720A4C194FF}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$D$13</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>FUTILITY_PRUNING</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent3"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$A$14:$A$17</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>0.1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$D$14:$D$17</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>3.431748825307587</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3.3844054130674119</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3.3554284376216401</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3.3335566591855015</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-BD17-4B80-85E9-6720A4C194FF}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$E$13</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>SEE</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent4"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$A$14:$A$17</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>0.1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$E$14:$E$17</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>3.4194151546719214</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3.3824990761269986</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3.3459976090846211</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3.3366150512158277</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000004-BD17-4B80-85E9-6720A4C194FF}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$F$13</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>NEW_FUTILITY</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent5"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent5"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent5"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$A$14:$A$17</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>0.1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$F$14:$F$17</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="4"/>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000005-BD17-4B80-85E9-6720A4C194FF}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="5"/>
+          <c:order val="5"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$G$13</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>RAW_EVAL</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent6"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent6"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent6"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$A$14:$A$17</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>0.1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$G$14:$G$17</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>3.5661604002063623</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3.5661604002063623</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3.5661604002063623</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3.5661604002063623</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000006-BD17-4B80-85E9-6720A4C194FF}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="6"/>
+          <c:order val="6"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$H$13</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>NULLWINDOW_NULLMOVE</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1">
+                    <a:lumMod val="60000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$A$14:$A$17</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>0.1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$H$14:$H$17</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>3.4144399247900088</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3.3665263997182615</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3.3352661063249514</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3.3161121814558685</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000007-BD17-4B80-85E9-6720A4C194FF}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -335,11 +804,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="718517311"/>
-        <c:axId val="718515231"/>
+        <c:axId val="452302560"/>
+        <c:axId val="452302976"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="718517311"/>
+        <c:axId val="452302560"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -396,12 +865,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="718515231"/>
+        <c:crossAx val="452302976"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="718515231"/>
+        <c:axId val="452302976"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -458,7 +927,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="718517311"/>
+        <c:crossAx val="452302560"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1106,22 +1575,22 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>590550</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>52387</xdr:rowOff>
+      <xdr:colOff>66674</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>90487</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>19</xdr:col>
-      <xdr:colOff>257175</xdr:colOff>
-      <xdr:row>30</xdr:row>
-      <xdr:rowOff>128587</xdr:rowOff>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>114299</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>123825</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="3" name="Chart 2">
+        <xdr:cNvPr id="4" name="Chart 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D2E5C361-03B6-4C51-826F-A008C75C2D53}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{601C3E75-B83C-4522-B1C0-A346D67990A7}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1439,10 +1908,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2E2554D6-BC87-453B-B54D-B4CC9ADCBBAB}">
-  <dimension ref="A1:V17"/>
+  <dimension ref="A1:V19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11:D11"/>
+      <selection activeCell="H24" sqref="H24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1451,6 +1920,10 @@
     <col min="2" max="2" width="17.42578125" customWidth="1"/>
     <col min="3" max="3" width="10.28515625" customWidth="1"/>
     <col min="4" max="4" width="17.85546875" customWidth="1"/>
+    <col min="5" max="5" width="18.28515625" customWidth="1"/>
+    <col min="6" max="6" width="18.85546875" customWidth="1"/>
+    <col min="7" max="7" width="11" customWidth="1"/>
+    <col min="8" max="8" width="24.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:22" x14ac:dyDescent="0.25">
@@ -1463,52 +1936,100 @@
       <c r="D1" t="s">
         <v>4</v>
       </c>
+      <c r="E1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H1" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="2" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="B2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D2">
         <v>1</v>
+      </c>
+      <c r="E2">
+        <v>0</v>
+      </c>
+      <c r="F2">
+        <v>1</v>
+      </c>
+      <c r="G2">
+        <v>0</v>
+      </c>
+      <c r="H2">
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="B3">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="C3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D3">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="E3">
+        <v>1</v>
+      </c>
+      <c r="F3">
+        <v>1</v>
+      </c>
+      <c r="G3">
+        <v>1</v>
+      </c>
+      <c r="H3">
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B4">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="C4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D4">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="E4">
+        <v>0</v>
+      </c>
+      <c r="F4">
+        <v>1</v>
+      </c>
+      <c r="G4">
+        <v>1</v>
+      </c>
+      <c r="H4">
+        <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B5">
         <v>10</v>
@@ -1517,12 +2038,24 @@
         <v>0</v>
       </c>
       <c r="D5">
+        <v>0</v>
+      </c>
+      <c r="E5">
+        <v>0</v>
+      </c>
+      <c r="F5">
+        <v>0</v>
+      </c>
+      <c r="G5">
+        <v>10</v>
+      </c>
+      <c r="H5">
         <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B6">
         <v>10</v>
@@ -1533,171 +2066,339 @@
       <c r="D6">
         <v>0</v>
       </c>
+      <c r="E6">
+        <v>0</v>
+      </c>
+      <c r="F6">
+        <v>0</v>
+      </c>
+      <c r="G6">
+        <v>10</v>
+      </c>
+      <c r="H6">
+        <v>0</v>
+      </c>
     </row>
     <row r="7" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A7">
-        <v>0.1</v>
+      <c r="A7" t="s">
+        <v>8</v>
       </c>
       <c r="B7">
-        <v>117799</v>
+        <v>10</v>
       </c>
       <c r="C7">
-        <v>117606</v>
+        <v>0</v>
       </c>
       <c r="D7">
-        <v>117769</v>
+        <v>0</v>
+      </c>
+      <c r="E7">
+        <v>0</v>
+      </c>
+      <c r="F7">
+        <v>0</v>
+      </c>
+      <c r="G7">
+        <v>10</v>
+      </c>
+      <c r="H7">
+        <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A8">
-        <v>0.5</v>
+      <c r="A8" t="s">
+        <v>9</v>
       </c>
       <c r="B8">
-        <v>113807</v>
+        <v>10</v>
       </c>
       <c r="C8">
-        <v>113680</v>
+        <v>0</v>
       </c>
       <c r="D8">
-        <v>114542</v>
+        <v>0</v>
+      </c>
+      <c r="E8">
+        <v>0</v>
+      </c>
+      <c r="F8">
+        <v>0</v>
+      </c>
+      <c r="G8">
+        <v>10</v>
+      </c>
+      <c r="H8">
+        <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A9">
-        <v>1</v>
+        <v>0.1</v>
       </c>
       <c r="B9">
-        <v>112868</v>
+        <v>117799</v>
       </c>
       <c r="C9">
-        <v>111013</v>
+        <v>117606</v>
       </c>
       <c r="D9">
-        <v>112589</v>
+        <v>117769</v>
+      </c>
+      <c r="E9">
+        <v>116924</v>
+      </c>
+      <c r="F9">
+        <v>116634</v>
+      </c>
+      <c r="G9">
+        <v>127175</v>
+      </c>
+      <c r="H9">
+        <v>116584</v>
       </c>
     </row>
     <row r="10" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A10">
-        <v>3</v>
+        <v>0.5</v>
       </c>
       <c r="B10">
-        <v>110773</v>
+        <v>113807</v>
       </c>
       <c r="C10">
-        <v>108053</v>
+        <v>113680</v>
       </c>
       <c r="D10">
-        <v>111126</v>
+        <v>114542</v>
+      </c>
+      <c r="E10">
+        <v>114413</v>
+      </c>
+      <c r="G10">
+        <v>127175</v>
+      </c>
+      <c r="H10">
+        <v>113335</v>
       </c>
     </row>
     <row r="11" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="B11" t="s">
-        <v>0</v>
-      </c>
-      <c r="C11" t="s">
+      <c r="A11">
         <v>1</v>
       </c>
-      <c r="D11" t="s">
-        <v>4</v>
+      <c r="B11">
+        <v>112868</v>
+      </c>
+      <c r="C11">
+        <v>111013</v>
+      </c>
+      <c r="D11">
+        <v>112589</v>
+      </c>
+      <c r="E11">
+        <v>111957</v>
+      </c>
+      <c r="G11">
+        <v>127175</v>
+      </c>
+      <c r="H11">
+        <v>111240</v>
       </c>
     </row>
     <row r="12" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A12">
-        <v>0.1</v>
-      </c>
-      <c r="B12" s="3">
-        <f>SQRT(B7) / 100</f>
-        <v>3.4321858924015176</v>
-      </c>
-      <c r="C12" s="3">
-        <f>SQRT(C7) / 100</f>
-        <v>3.4293731205571669</v>
-      </c>
-      <c r="D12" s="3">
-        <f>SQRT(D7) / 100</f>
-        <v>3.431748825307587</v>
-      </c>
-      <c r="E12" s="2"/>
-      <c r="F12" s="2"/>
-      <c r="G12" s="2"/>
-      <c r="H12" s="2"/>
-      <c r="I12" s="2"/>
-      <c r="J12" s="2"/>
-      <c r="K12" s="2"/>
-      <c r="L12" s="2"/>
-      <c r="M12" s="2"/>
-      <c r="N12" s="2"/>
-      <c r="O12" s="2"/>
-      <c r="P12" s="2"/>
-      <c r="Q12" s="2"/>
-      <c r="R12" s="2"/>
-      <c r="S12" s="2"/>
-      <c r="T12" s="2"/>
-      <c r="U12" s="2"/>
-      <c r="V12" s="2"/>
+        <v>3</v>
+      </c>
+      <c r="B12">
+        <v>110773</v>
+      </c>
+      <c r="C12">
+        <v>108053</v>
+      </c>
+      <c r="D12">
+        <v>111126</v>
+      </c>
+      <c r="E12">
+        <v>111330</v>
+      </c>
+      <c r="G12">
+        <v>127175</v>
+      </c>
+      <c r="H12">
+        <v>109966</v>
+      </c>
     </row>
     <row r="13" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A13">
-        <v>0.5</v>
-      </c>
-      <c r="B13" s="3">
-        <f t="shared" ref="B13:C15" si="0">SQRT(B8) / 100</f>
-        <v>3.3735293091953418</v>
-      </c>
-      <c r="C13" s="3">
-        <f t="shared" si="0"/>
-        <v>3.3716464820618426</v>
-      </c>
-      <c r="D13" s="3">
-        <f t="shared" ref="D13" si="1">SQRT(D8) / 100</f>
-        <v>3.3844054130674119</v>
+      <c r="B13" t="s">
+        <v>0</v>
+      </c>
+      <c r="C13" t="s">
+        <v>1</v>
+      </c>
+      <c r="D13" t="s">
+        <v>4</v>
+      </c>
+      <c r="E13" t="s">
+        <v>11</v>
+      </c>
+      <c r="F13" t="s">
+        <v>13</v>
+      </c>
+      <c r="G13" t="s">
+        <v>14</v>
+      </c>
+      <c r="H13" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="14" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A14">
-        <v>1</v>
+        <v>0.1</v>
       </c>
       <c r="B14" s="3">
+        <f>SQRT(B9) / 100</f>
+        <v>3.4321858924015176</v>
+      </c>
+      <c r="C14" s="3">
+        <f>SQRT(C9) / 100</f>
+        <v>3.4293731205571669</v>
+      </c>
+      <c r="D14" s="3">
+        <f>SQRT(D9) / 100</f>
+        <v>3.431748825307587</v>
+      </c>
+      <c r="E14" s="3">
+        <f>SQRT(E9) / 100</f>
+        <v>3.4194151546719214</v>
+      </c>
+      <c r="F14" s="3"/>
+      <c r="G14" s="3">
+        <f t="shared" ref="F14:H17" si="0">SQRT(G9) / 100</f>
+        <v>3.5661604002063623</v>
+      </c>
+      <c r="H14" s="3">
         <f t="shared" si="0"/>
-        <v>3.3595833074951424</v>
-      </c>
-      <c r="C14" s="3">
-        <f t="shared" si="0"/>
-        <v>3.3318613416527403</v>
-      </c>
-      <c r="D14" s="3">
-        <f t="shared" ref="D14" si="2">SQRT(D9) / 100</f>
-        <v>3.3554284376216401</v>
-      </c>
+        <v>3.4144399247900088</v>
+      </c>
+      <c r="I14" s="2"/>
+      <c r="J14" s="2"/>
+      <c r="K14" s="2"/>
+      <c r="L14" s="2"/>
+      <c r="M14" s="2"/>
+      <c r="N14" s="2"/>
+      <c r="O14" s="2"/>
+      <c r="P14" s="2"/>
+      <c r="Q14" s="2"/>
+      <c r="R14" s="2"/>
+      <c r="S14" s="2"/>
+      <c r="T14" s="2"/>
+      <c r="U14" s="2"/>
+      <c r="V14" s="2"/>
     </row>
     <row r="15" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A15">
+        <v>0.5</v>
+      </c>
+      <c r="B15" s="3">
+        <f t="shared" ref="B15:C17" si="1">SQRT(B10) / 100</f>
+        <v>3.3735293091953418</v>
+      </c>
+      <c r="C15" s="3">
+        <f t="shared" si="1"/>
+        <v>3.3716464820618426</v>
+      </c>
+      <c r="D15" s="3">
+        <f t="shared" ref="D15:E15" si="2">SQRT(D10) / 100</f>
+        <v>3.3844054130674119</v>
+      </c>
+      <c r="E15" s="3">
+        <f t="shared" si="2"/>
+        <v>3.3824990761269986</v>
+      </c>
+      <c r="F15" s="3"/>
+      <c r="G15" s="3">
+        <f t="shared" ref="F15:H15" si="3">SQRT(G10) / 100</f>
+        <v>3.5661604002063623</v>
+      </c>
+      <c r="H15" s="3">
+        <f t="shared" si="0"/>
+        <v>3.3665263997182615</v>
+      </c>
+    </row>
+    <row r="16" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>1</v>
+      </c>
+      <c r="B16" s="3">
+        <f t="shared" si="1"/>
+        <v>3.3595833074951424</v>
+      </c>
+      <c r="C16" s="3">
+        <f t="shared" si="1"/>
+        <v>3.3318613416527403</v>
+      </c>
+      <c r="D16" s="3">
+        <f t="shared" ref="D16:E16" si="4">SQRT(D11) / 100</f>
+        <v>3.3554284376216401</v>
+      </c>
+      <c r="E16" s="3">
+        <f t="shared" si="4"/>
+        <v>3.3459976090846211</v>
+      </c>
+      <c r="F16" s="3"/>
+      <c r="G16" s="3">
+        <f t="shared" ref="F16:H16" si="5">SQRT(G11) / 100</f>
+        <v>3.5661604002063623</v>
+      </c>
+      <c r="H16" s="3">
+        <f t="shared" si="0"/>
+        <v>3.3352661063249514</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A17">
         <v>3</v>
       </c>
-      <c r="B15" s="3">
+      <c r="B17" s="3">
+        <f t="shared" si="1"/>
+        <v>3.3282578025147029</v>
+      </c>
+      <c r="C17" s="3">
+        <f t="shared" si="1"/>
+        <v>3.2871416154464659</v>
+      </c>
+      <c r="D17" s="3">
+        <f t="shared" ref="D17:E17" si="6">SQRT(D12) / 100</f>
+        <v>3.3335566591855015</v>
+      </c>
+      <c r="E17" s="3">
+        <f t="shared" si="6"/>
+        <v>3.3366150512158277</v>
+      </c>
+      <c r="F17" s="3"/>
+      <c r="G17" s="3">
+        <f t="shared" ref="F17:H17" si="7">SQRT(G12) / 100</f>
+        <v>3.5661604002063623</v>
+      </c>
+      <c r="H17" s="3">
         <f t="shared" si="0"/>
-        <v>3.3282578025147029</v>
-      </c>
-      <c r="C15" s="3">
-        <f t="shared" si="0"/>
-        <v>3.2871416154464659</v>
-      </c>
-      <c r="D15" s="3">
-        <f t="shared" ref="D15" si="3">SQRT(D10) / 100</f>
-        <v>3.3335566591855015</v>
+        <v>3.3161121814558685</v>
       </c>
     </row>
-    <row r="17" spans="1:4" ht="75" x14ac:dyDescent="0.25">
-      <c r="A17" s="2" t="s">
+    <row r="19" spans="1:8" ht="90" x14ac:dyDescent="0.25">
+      <c r="A19" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B17" s="1" t="s">
+      <c r="B19" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C17" s="1" t="s">
+      <c r="C19" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D17" s="2"/>
+      <c r="D19" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>10</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
refactored out futility pruning, added depth-2 futility pruning
</commit_message>
<xml_diff>
--- a/src/regressions.xlsx
+++ b/src/regressions.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\github\chess\viridithas_chess\src\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A58FDF5-D365-4FCE-A3EA-D4694AC2DE1D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F263AE1-CECB-4FB3-9070-C68959D7813C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{D29FE3B1-2868-4402-B04C-E409A12BF9BB}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="18">
   <si>
     <t>ALL_COMPONENTS</t>
   </si>
@@ -82,6 +82,12 @@
   </si>
   <si>
     <t>NULLWINDOW_NULLMOVE</t>
+  </si>
+  <si>
+    <t>NULLMOVE</t>
+  </si>
+  <si>
+    <t>DEEP_FUTILITY</t>
   </si>
 </sst>
 </file>
@@ -198,7 +204,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$B$13</c:f>
+              <c:f>Sheet1!$B$21</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -233,7 +239,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$A$14:$A$17</c:f>
+              <c:f>Sheet1!$A$22:$A$25</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
@@ -254,7 +260,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$B$14:$B$17</c:f>
+              <c:f>Sheet1!$B$22:$B$25</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="4"/>
@@ -285,7 +291,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$C$13</c:f>
+              <c:f>Sheet1!$C$21</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -320,7 +326,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$A$14:$A$17</c:f>
+              <c:f>Sheet1!$A$22:$A$25</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
@@ -341,7 +347,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$C$14:$C$17</c:f>
+              <c:f>Sheet1!$C$22:$C$25</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="4"/>
@@ -372,7 +378,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$D$13</c:f>
+              <c:f>Sheet1!$D$21</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -407,7 +413,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$A$14:$A$17</c:f>
+              <c:f>Sheet1!$A$22:$A$25</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
@@ -428,7 +434,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$D$14:$D$17</c:f>
+              <c:f>Sheet1!$D$22:$D$25</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="4"/>
@@ -459,7 +465,7 @@
           <c:order val="3"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$E$13</c:f>
+              <c:f>Sheet1!$E$21</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -494,7 +500,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$A$14:$A$17</c:f>
+              <c:f>Sheet1!$A$22:$A$25</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
@@ -515,7 +521,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$E$14:$E$17</c:f>
+              <c:f>Sheet1!$E$22:$E$25</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="4"/>
@@ -546,7 +552,7 @@
           <c:order val="4"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$F$13</c:f>
+              <c:f>Sheet1!$F$21</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -581,7 +587,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$A$14:$A$17</c:f>
+              <c:f>Sheet1!$A$22:$A$25</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
@@ -602,10 +608,22 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$F$14:$F$17</c:f>
+              <c:f>Sheet1!$F$22:$F$25</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>3.4151720308060618</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3.3399550895184205</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3.3297597510931625</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3.3143325119848792</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
@@ -621,7 +639,7 @@
           <c:order val="5"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$G$13</c:f>
+              <c:f>Sheet1!$G$21</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -656,7 +674,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$A$14:$A$17</c:f>
+              <c:f>Sheet1!$A$22:$A$25</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
@@ -677,7 +695,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$G$14:$G$17</c:f>
+              <c:f>Sheet1!$G$22:$G$25</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="4"/>
@@ -708,7 +726,7 @@
           <c:order val="6"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$H$13</c:f>
+              <c:f>Sheet1!$H$21</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -749,7 +767,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$A$14:$A$17</c:f>
+              <c:f>Sheet1!$A$22:$A$25</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
@@ -770,7 +788,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$H$14:$H$17</c:f>
+              <c:f>Sheet1!$H$22:$H$25</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="4"/>
@@ -1576,12 +1594,12 @@
     <xdr:from>
       <xdr:col>10</xdr:col>
       <xdr:colOff>66674</xdr:colOff>
-      <xdr:row>7</xdr:row>
-      <xdr:rowOff>90487</xdr:rowOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>20</xdr:col>
-      <xdr:colOff>114299</xdr:colOff>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>161925</xdr:colOff>
       <xdr:row>24</xdr:row>
       <xdr:rowOff>123825</xdr:rowOff>
     </xdr:to>
@@ -1908,10 +1926,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2E2554D6-BC87-453B-B54D-B4CC9ADCBBAB}">
-  <dimension ref="A1:V19"/>
+  <dimension ref="A1:V27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H24" sqref="H24"/>
+      <selection activeCell="I21" sqref="I21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1924,6 +1942,7 @@
     <col min="6" max="6" width="18.85546875" customWidth="1"/>
     <col min="7" max="7" width="11" customWidth="1"/>
     <col min="8" max="8" width="24.28515625" customWidth="1"/>
+    <col min="9" max="9" width="20.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:22" x14ac:dyDescent="0.25">
@@ -1948,6 +1967,9 @@
       <c r="H1" t="s">
         <v>15</v>
       </c>
+      <c r="I1" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="2" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
@@ -1974,6 +1996,9 @@
       <c r="H2">
         <v>0</v>
       </c>
+      <c r="I2">
+        <v>2</v>
+      </c>
     </row>
     <row r="3" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
@@ -2000,6 +2025,9 @@
       <c r="H3">
         <v>1</v>
       </c>
+      <c r="I3">
+        <v>1</v>
+      </c>
     </row>
     <row r="4" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
@@ -2026,6 +2054,9 @@
       <c r="H4">
         <v>1</v>
       </c>
+      <c r="I4">
+        <v>1</v>
+      </c>
     </row>
     <row r="5" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
@@ -2052,6 +2083,9 @@
       <c r="H5">
         <v>0</v>
       </c>
+      <c r="I5">
+        <v>0</v>
+      </c>
     </row>
     <row r="6" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
@@ -2078,6 +2112,9 @@
       <c r="H6">
         <v>0</v>
       </c>
+      <c r="I6">
+        <v>0</v>
+      </c>
     </row>
     <row r="7" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
@@ -2104,6 +2141,9 @@
       <c r="H7">
         <v>0</v>
       </c>
+      <c r="I7">
+        <v>0</v>
+      </c>
     </row>
     <row r="8" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
@@ -2130,154 +2170,40 @@
       <c r="H8">
         <v>0</v>
       </c>
+      <c r="I8">
+        <v>0</v>
+      </c>
     </row>
     <row r="9" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A9">
-        <v>0.1</v>
+      <c r="A9" t="s">
+        <v>16</v>
       </c>
       <c r="B9">
-        <v>117799</v>
+        <v>1</v>
       </c>
       <c r="C9">
-        <v>117606</v>
+        <v>1</v>
       </c>
       <c r="D9">
-        <v>117769</v>
+        <v>1</v>
       </c>
       <c r="E9">
-        <v>116924</v>
+        <v>1</v>
       </c>
       <c r="F9">
-        <v>116634</v>
+        <v>2</v>
       </c>
       <c r="G9">
-        <v>127175</v>
+        <v>0</v>
       </c>
       <c r="H9">
-        <v>116584</v>
-      </c>
-    </row>
-    <row r="10" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A10">
-        <v>0.5</v>
-      </c>
-      <c r="B10">
-        <v>113807</v>
-      </c>
-      <c r="C10">
-        <v>113680</v>
-      </c>
-      <c r="D10">
-        <v>114542</v>
-      </c>
-      <c r="E10">
-        <v>114413</v>
-      </c>
-      <c r="G10">
-        <v>127175</v>
-      </c>
-      <c r="H10">
-        <v>113335</v>
-      </c>
-    </row>
-    <row r="11" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A11">
-        <v>1</v>
-      </c>
-      <c r="B11">
-        <v>112868</v>
-      </c>
-      <c r="C11">
-        <v>111013</v>
-      </c>
-      <c r="D11">
-        <v>112589</v>
-      </c>
-      <c r="E11">
-        <v>111957</v>
-      </c>
-      <c r="G11">
-        <v>127175</v>
-      </c>
-      <c r="H11">
-        <v>111240</v>
-      </c>
-    </row>
-    <row r="12" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A12">
-        <v>3</v>
-      </c>
-      <c r="B12">
-        <v>110773</v>
-      </c>
-      <c r="C12">
-        <v>108053</v>
-      </c>
-      <c r="D12">
-        <v>111126</v>
-      </c>
-      <c r="E12">
-        <v>111330</v>
-      </c>
-      <c r="G12">
-        <v>127175</v>
-      </c>
-      <c r="H12">
-        <v>109966</v>
-      </c>
-    </row>
-    <row r="13" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="B13" t="s">
-        <v>0</v>
-      </c>
-      <c r="C13" t="s">
-        <v>1</v>
-      </c>
-      <c r="D13" t="s">
-        <v>4</v>
-      </c>
-      <c r="E13" t="s">
-        <v>11</v>
-      </c>
-      <c r="F13" t="s">
-        <v>13</v>
-      </c>
-      <c r="G13" t="s">
-        <v>14</v>
-      </c>
-      <c r="H13" t="s">
-        <v>15</v>
+        <v>2</v>
+      </c>
+      <c r="I9">
+        <v>2</v>
       </c>
     </row>
     <row r="14" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A14">
-        <v>0.1</v>
-      </c>
-      <c r="B14" s="3">
-        <f>SQRT(B9) / 100</f>
-        <v>3.4321858924015176</v>
-      </c>
-      <c r="C14" s="3">
-        <f>SQRT(C9) / 100</f>
-        <v>3.4293731205571669</v>
-      </c>
-      <c r="D14" s="3">
-        <f>SQRT(D9) / 100</f>
-        <v>3.431748825307587</v>
-      </c>
-      <c r="E14" s="3">
-        <f>SQRT(E9) / 100</f>
-        <v>3.4194151546719214</v>
-      </c>
-      <c r="F14" s="3"/>
-      <c r="G14" s="3">
-        <f t="shared" ref="F14:H17" si="0">SQRT(G9) / 100</f>
-        <v>3.5661604002063623</v>
-      </c>
-      <c r="H14" s="3">
-        <f t="shared" si="0"/>
-        <v>3.4144399247900088</v>
-      </c>
       <c r="I14" s="2"/>
       <c r="J14" s="2"/>
       <c r="K14" s="2"/>
@@ -2293,110 +2219,282 @@
       <c r="U14" s="2"/>
       <c r="V14" s="2"/>
     </row>
-    <row r="15" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A15">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>0.1</v>
+      </c>
+      <c r="B17">
+        <v>117799</v>
+      </c>
+      <c r="C17">
+        <v>117606</v>
+      </c>
+      <c r="D17">
+        <v>117769</v>
+      </c>
+      <c r="E17">
+        <v>116924</v>
+      </c>
+      <c r="F17">
+        <v>116634</v>
+      </c>
+      <c r="G17">
+        <v>127175</v>
+      </c>
+      <c r="H17">
+        <v>116584</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A18">
         <v>0.5</v>
       </c>
-      <c r="B15" s="3">
-        <f t="shared" ref="B15:C17" si="1">SQRT(B10) / 100</f>
+      <c r="B18">
+        <v>113807</v>
+      </c>
+      <c r="C18">
+        <v>113680</v>
+      </c>
+      <c r="D18">
+        <v>114542</v>
+      </c>
+      <c r="E18">
+        <v>114413</v>
+      </c>
+      <c r="F18">
+        <v>111553</v>
+      </c>
+      <c r="G18">
+        <v>127175</v>
+      </c>
+      <c r="H18">
+        <v>113335</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>1</v>
+      </c>
+      <c r="B19">
+        <v>112868</v>
+      </c>
+      <c r="C19">
+        <v>111013</v>
+      </c>
+      <c r="D19">
+        <v>112589</v>
+      </c>
+      <c r="E19">
+        <v>111957</v>
+      </c>
+      <c r="F19">
+        <v>110873</v>
+      </c>
+      <c r="G19">
+        <v>127175</v>
+      </c>
+      <c r="H19">
+        <v>111240</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>3</v>
+      </c>
+      <c r="B20">
+        <v>110773</v>
+      </c>
+      <c r="C20">
+        <v>108053</v>
+      </c>
+      <c r="D20">
+        <v>111126</v>
+      </c>
+      <c r="E20">
+        <v>111330</v>
+      </c>
+      <c r="F20">
+        <v>109848</v>
+      </c>
+      <c r="G20">
+        <v>127175</v>
+      </c>
+      <c r="H20">
+        <v>109966</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B21" t="s">
+        <v>0</v>
+      </c>
+      <c r="C21" t="s">
+        <v>1</v>
+      </c>
+      <c r="D21" t="s">
+        <v>4</v>
+      </c>
+      <c r="E21" t="s">
+        <v>11</v>
+      </c>
+      <c r="F21" t="s">
+        <v>13</v>
+      </c>
+      <c r="G21" t="s">
+        <v>14</v>
+      </c>
+      <c r="H21" t="s">
+        <v>15</v>
+      </c>
+      <c r="I21" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>0.1</v>
+      </c>
+      <c r="B22" s="3">
+        <f>SQRT(B17) / 100</f>
+        <v>3.4321858924015176</v>
+      </c>
+      <c r="C22" s="3">
+        <f>SQRT(C17) / 100</f>
+        <v>3.4293731205571669</v>
+      </c>
+      <c r="D22" s="3">
+        <f>SQRT(D17) / 100</f>
+        <v>3.431748825307587</v>
+      </c>
+      <c r="E22" s="3">
+        <f>SQRT(E17) / 100</f>
+        <v>3.4194151546719214</v>
+      </c>
+      <c r="F22" s="3">
+        <f>SQRT(F17) / 100</f>
+        <v>3.4151720308060618</v>
+      </c>
+      <c r="G22" s="3">
+        <f t="shared" ref="F22:H25" si="0">SQRT(G17) / 100</f>
+        <v>3.5661604002063623</v>
+      </c>
+      <c r="H22" s="3">
+        <f t="shared" si="0"/>
+        <v>3.4144399247900088</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>0.5</v>
+      </c>
+      <c r="B23" s="3">
+        <f t="shared" ref="B23:C25" si="1">SQRT(B18) / 100</f>
         <v>3.3735293091953418</v>
       </c>
-      <c r="C15" s="3">
+      <c r="C23" s="3">
         <f t="shared" si="1"/>
         <v>3.3716464820618426</v>
       </c>
-      <c r="D15" s="3">
-        <f t="shared" ref="D15:E15" si="2">SQRT(D10) / 100</f>
+      <c r="D23" s="3">
+        <f t="shared" ref="D23:E23" si="2">SQRT(D18) / 100</f>
         <v>3.3844054130674119</v>
       </c>
-      <c r="E15" s="3">
+      <c r="E23" s="3">
         <f t="shared" si="2"/>
         <v>3.3824990761269986</v>
       </c>
-      <c r="F15" s="3"/>
-      <c r="G15" s="3">
-        <f t="shared" ref="F15:H15" si="3">SQRT(G10) / 100</f>
+      <c r="F23" s="3">
+        <f>SQRT(F18) / 100</f>
+        <v>3.3399550895184205</v>
+      </c>
+      <c r="G23" s="3">
+        <f t="shared" ref="F23:H23" si="3">SQRT(G18) / 100</f>
         <v>3.5661604002063623</v>
       </c>
-      <c r="H15" s="3">
+      <c r="H23" s="3">
         <f t="shared" si="0"/>
         <v>3.3665263997182615</v>
       </c>
     </row>
-    <row r="16" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A16">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A24">
         <v>1</v>
       </c>
-      <c r="B16" s="3">
+      <c r="B24" s="3">
         <f t="shared" si="1"/>
         <v>3.3595833074951424</v>
       </c>
-      <c r="C16" s="3">
+      <c r="C24" s="3">
         <f t="shared" si="1"/>
         <v>3.3318613416527403</v>
       </c>
-      <c r="D16" s="3">
-        <f t="shared" ref="D16:E16" si="4">SQRT(D11) / 100</f>
+      <c r="D24" s="3">
+        <f t="shared" ref="D24:E24" si="4">SQRT(D19) / 100</f>
         <v>3.3554284376216401</v>
       </c>
-      <c r="E16" s="3">
+      <c r="E24" s="3">
         <f t="shared" si="4"/>
         <v>3.3459976090846211</v>
       </c>
-      <c r="F16" s="3"/>
-      <c r="G16" s="3">
-        <f t="shared" ref="F16:H16" si="5">SQRT(G11) / 100</f>
+      <c r="F24" s="3">
+        <f>SQRT(F19) / 100</f>
+        <v>3.3297597510931625</v>
+      </c>
+      <c r="G24" s="3">
+        <f t="shared" ref="F24:H24" si="5">SQRT(G19) / 100</f>
         <v>3.5661604002063623</v>
       </c>
-      <c r="H16" s="3">
+      <c r="H24" s="3">
         <f t="shared" si="0"/>
         <v>3.3352661063249514</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A17">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A25">
         <v>3</v>
       </c>
-      <c r="B17" s="3">
+      <c r="B25" s="3">
         <f t="shared" si="1"/>
         <v>3.3282578025147029</v>
       </c>
-      <c r="C17" s="3">
+      <c r="C25" s="3">
         <f t="shared" si="1"/>
         <v>3.2871416154464659</v>
       </c>
-      <c r="D17" s="3">
-        <f t="shared" ref="D17:E17" si="6">SQRT(D12) / 100</f>
+      <c r="D25" s="3">
+        <f t="shared" ref="D25:E25" si="6">SQRT(D20) / 100</f>
         <v>3.3335566591855015</v>
       </c>
-      <c r="E17" s="3">
+      <c r="E25" s="3">
         <f t="shared" si="6"/>
         <v>3.3366150512158277</v>
       </c>
-      <c r="F17" s="3"/>
-      <c r="G17" s="3">
-        <f t="shared" ref="F17:H17" si="7">SQRT(G12) / 100</f>
+      <c r="F25" s="3">
+        <f>SQRT(F20) / 100</f>
+        <v>3.3143325119848792</v>
+      </c>
+      <c r="G25" s="3">
+        <f t="shared" ref="F25:H25" si="7">SQRT(G20) / 100</f>
         <v>3.5661604002063623</v>
       </c>
-      <c r="H17" s="3">
+      <c r="H25" s="3">
         <f t="shared" si="0"/>
         <v>3.3161121814558685</v>
       </c>
     </row>
-    <row r="19" spans="1:8" ht="90" x14ac:dyDescent="0.25">
-      <c r="A19" s="2" t="s">
+    <row r="27" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+      <c r="A27" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B19" s="1" t="s">
+      <c r="B27" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C19" s="1" t="s">
+      <c r="C27" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D19" s="1" t="s">
+      <c r="D27" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="E19" s="1" t="s">
+      <c r="E27" s="1" t="s">
         <v>10</v>
       </c>
     </row>

</xml_diff>